<commit_message>
updated new ramadan times
</commit_message>
<xml_diff>
--- a/public/datas/dhaka.xlsx
+++ b/public/datas/dhaka.xlsx
@@ -16,220 +16,220 @@
     <t>2023-03-24</t>
   </si>
   <si>
-    <t>04:41 AM</t>
+    <t>04:38 AM</t>
   </si>
   <si>
-    <t>06:11 PM</t>
+    <t>06:14 PM</t>
   </si>
   <si>
     <t>2023-03-25</t>
   </si>
   <si>
-    <t>04:40 AM</t>
-  </si>
-  <si>
-    <t>06:12 PM</t>
+    <t>04:37 AM</t>
   </si>
   <si>
     <t>2023-03-26</t>
   </si>
   <si>
-    <t>04:39 AM</t>
+    <t>04:36 AM</t>
+  </si>
+  <si>
+    <t>06:15 PM</t>
   </si>
   <si>
     <t>2023-03-27</t>
   </si>
   <si>
-    <t>04:38 AM</t>
-  </si>
-  <si>
-    <t>06:13 PM</t>
+    <t>04:35 AM</t>
   </si>
   <si>
     <t>2023-03-28</t>
   </si>
   <si>
-    <t>04:37 AM</t>
+    <t>04:34 AM</t>
+  </si>
+  <si>
+    <t>06:16 PM</t>
   </si>
   <si>
     <t>2023-03-29</t>
   </si>
   <si>
-    <t>04:36 AM</t>
+    <t>04:32 AM</t>
   </si>
   <si>
     <t>2023-03-30</t>
   </si>
   <si>
-    <t>04:35 AM</t>
+    <t>04:31 AM</t>
   </si>
   <si>
-    <t>06:14 PM</t>
+    <t>06:17 PM</t>
   </si>
   <si>
     <t>2023-03-31</t>
   </si>
   <si>
-    <t>04:34 AM</t>
+    <t>04:30 AM</t>
   </si>
   <si>
     <t>2023-04-01</t>
   </si>
   <si>
-    <t>04:33 AM</t>
+    <t>04:29 AM</t>
+  </si>
+  <si>
+    <t>06:18 PM</t>
   </si>
   <si>
     <t>2023-04-02</t>
   </si>
   <si>
-    <t>04:32 AM</t>
-  </si>
-  <si>
-    <t>06:15 PM</t>
+    <t>04:28 AM</t>
   </si>
   <si>
     <t>2023-04-03</t>
   </si>
   <si>
-    <t>04:31 AM</t>
+    <t>04:27 AM</t>
+  </si>
+  <si>
+    <t>06:19 PM</t>
   </si>
   <si>
     <t>2023-04-04</t>
   </si>
   <si>
-    <t>04:29 AM</t>
-  </si>
-  <si>
-    <t>06:16 PM</t>
+    <t>04:26 AM</t>
   </si>
   <si>
     <t>2023-04-05</t>
   </si>
   <si>
-    <t>04:28 AM</t>
+    <t>04:25 AM</t>
+  </si>
+  <si>
+    <t>06:20 PM</t>
   </si>
   <si>
     <t>2023-04-06</t>
   </si>
   <si>
-    <t>04:27 AM</t>
+    <t>04:24 AM</t>
   </si>
   <si>
     <t>2023-04-07</t>
   </si>
   <si>
-    <t>04:26 AM</t>
+    <t>04:23 AM</t>
   </si>
   <si>
-    <t>06:17 PM</t>
+    <t>06:21 PM</t>
   </si>
   <si>
     <t>2023-04-08</t>
   </si>
   <si>
-    <t>04:25 AM</t>
+    <t>04:22 AM</t>
   </si>
   <si>
     <t>2023-04-09</t>
   </si>
   <si>
-    <t>04:24 AM</t>
+    <t>04:21 AM</t>
   </si>
   <si>
-    <t>06:18 PM</t>
+    <t>06:22 PM</t>
   </si>
   <si>
     <t>2023-04-10</t>
   </si>
   <si>
-    <t>04:23 AM</t>
+    <t>04:20 AM</t>
   </si>
   <si>
     <t>2023-04-11</t>
   </si>
   <si>
-    <t>04:22 AM</t>
+    <t>04:19 AM</t>
   </si>
   <si>
     <t>2023-04-12</t>
   </si>
   <si>
-    <t>04:21 AM</t>
+    <t>04:18 AM</t>
   </si>
   <si>
-    <t>06:19 PM</t>
+    <t>06:23 PM</t>
   </si>
   <si>
     <t>2023-04-13</t>
   </si>
   <si>
-    <t>04:20 AM</t>
+    <t>04:16 AM</t>
   </si>
   <si>
     <t>2023-04-14</t>
   </si>
   <si>
-    <t>04:19 AM</t>
-  </si>
-  <si>
-    <t>06:20 PM</t>
+    <t>04:15 AM</t>
   </si>
   <si>
     <t>2023-04-15</t>
   </si>
   <si>
-    <t>04:18 AM</t>
+    <t>04:14 AM</t>
+  </si>
+  <si>
+    <t>06:24 PM</t>
   </si>
   <si>
     <t>2023-04-16</t>
   </si>
   <si>
-    <t>04:17 AM</t>
+    <t>04:13 AM</t>
   </si>
   <si>
     <t>2023-04-17</t>
   </si>
   <si>
-    <t>04:16 AM</t>
-  </si>
-  <si>
-    <t>06:21 PM</t>
+    <t>04:12 AM</t>
   </si>
   <si>
     <t>2023-04-18</t>
   </si>
   <si>
-    <t>04:14 AM</t>
+    <t>04:11 AM</t>
+  </si>
+  <si>
+    <t>06:25 PM</t>
   </si>
   <si>
     <t>2023-04-19</t>
   </si>
   <si>
-    <t>04:13 AM</t>
-  </si>
-  <si>
-    <t>06:22 PM</t>
+    <t>04:10 AM</t>
   </si>
   <si>
     <t>2023-04-20</t>
   </si>
   <si>
-    <t>04:12 AM</t>
+    <t>04:09 AM</t>
+  </si>
+  <si>
+    <t>06:26 PM</t>
   </si>
   <si>
     <t>2023-04-21</t>
   </si>
   <si>
-    <t>04:11 AM</t>
-  </si>
-  <si>
-    <t>06:23 PM</t>
+    <t>04:08 AM</t>
   </si>
   <si>
     <t>2023-04-22</t>
   </si>
   <si>
-    <t>04:10 AM</t>
+    <t>04:07 AM</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -557,13 +557,13 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -597,7 +597,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -625,13 +625,13 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -665,7 +665,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -767,7 +767,7 @@
         <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -795,13 +795,13 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -835,7 +835,7 @@
         <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -863,13 +863,13 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -903,7 +903,7 @@
         <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -931,13 +931,13 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -965,13 +965,13 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -999,13 +999,13 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1033,13 +1033,13 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1067,13 +1067,13 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1101,13 +1101,13 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1135,13 +1135,13 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1169,13 +1169,13 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -1203,13 +1203,13 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1243,7 +1243,7 @@
         <v>55</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1271,13 +1271,13 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1305,13 +1305,13 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1345,7 +1345,7 @@
         <v>62</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1373,13 +1373,13 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1413,7 +1413,7 @@
         <v>67</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1441,13 +1441,13 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1481,7 +1481,7 @@
         <v>72</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>

</xml_diff>